<commit_message>
script with my correections
</commit_message>
<xml_diff>
--- a/data/add_factors.xlsx
+++ b/data/add_factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/fim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA63A15-9245-AB4C-90AF-52E3D54BF3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5577F356-1010-9E4E-A57A-72EBFB0ED8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19720" activeTab="4" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="2100" yWindow="500" windowWidth="33600" windowHeight="19720" activeTab="3" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -3602,21 +3602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3638,14 +3623,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -15189,68 +15189,68 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="381" t="s">
+      <c r="A2" s="376" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="381"/>
-      <c r="C2" s="381"/>
-      <c r="D2" s="381"/>
-      <c r="E2" s="381"/>
-      <c r="F2" s="381"/>
-      <c r="G2" s="381"/>
-      <c r="H2" s="381"/>
-      <c r="I2" s="381"/>
-      <c r="J2" s="381"/>
+      <c r="B2" s="376"/>
+      <c r="C2" s="376"/>
+      <c r="D2" s="376"/>
+      <c r="E2" s="376"/>
+      <c r="F2" s="376"/>
+      <c r="G2" s="376"/>
+      <c r="H2" s="376"/>
+      <c r="I2" s="376"/>
+      <c r="J2" s="376"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="381" t="s">
+      <c r="A3" s="376" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="381"/>
-      <c r="C3" s="381"/>
-      <c r="D3" s="381"/>
-      <c r="E3" s="381"/>
-      <c r="F3" s="381"/>
-      <c r="G3" s="381"/>
-      <c r="H3" s="381"/>
-      <c r="I3" s="381"/>
-      <c r="J3" s="381"/>
+      <c r="B3" s="376"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
+      <c r="G3" s="376"/>
+      <c r="H3" s="376"/>
+      <c r="I3" s="376"/>
+      <c r="J3" s="376"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="382"/>
-      <c r="B4" s="382"/>
-      <c r="C4" s="382"/>
-      <c r="D4" s="382"/>
-      <c r="E4" s="382"/>
-      <c r="F4" s="382"/>
-      <c r="G4" s="382"/>
-      <c r="H4" s="382"/>
-      <c r="I4" s="382"/>
-      <c r="J4" s="382"/>
-      <c r="K4" s="387" t="s">
+      <c r="A4" s="377"/>
+      <c r="B4" s="377"/>
+      <c r="C4" s="377"/>
+      <c r="D4" s="377"/>
+      <c r="E4" s="377"/>
+      <c r="F4" s="377"/>
+      <c r="G4" s="377"/>
+      <c r="H4" s="377"/>
+      <c r="I4" s="377"/>
+      <c r="J4" s="377"/>
+      <c r="K4" s="382" t="s">
         <v>159</v>
       </c>
-      <c r="L4" s="387"/>
-      <c r="M4" s="387"/>
-      <c r="N4" s="387"/>
+      <c r="L4" s="382"/>
+      <c r="M4" s="382"/>
+      <c r="N4" s="382"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="383" t="s">
+      <c r="C5" s="378" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="384"/>
-      <c r="E5" s="384"/>
-      <c r="F5" s="384"/>
-      <c r="G5" s="384"/>
-      <c r="H5" s="384"/>
-      <c r="I5" s="384"/>
-      <c r="J5" s="385"/>
+      <c r="D5" s="379"/>
+      <c r="E5" s="379"/>
+      <c r="F5" s="379"/>
+      <c r="G5" s="379"/>
+      <c r="H5" s="379"/>
+      <c r="I5" s="379"/>
+      <c r="J5" s="380"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="386" t="s">
+      <c r="L5" s="381" t="s">
         <v>106</v>
       </c>
       <c r="M5" s="352"/>
@@ -15261,16 +15261,16 @@
         <v>108</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="377">
+      <c r="C6" s="384">
         <v>2020</v>
       </c>
-      <c r="D6" s="378"/>
-      <c r="E6" s="378"/>
-      <c r="F6" s="378"/>
-      <c r="G6" s="378"/>
-      <c r="H6" s="378"/>
-      <c r="I6" s="378"/>
-      <c r="J6" s="379"/>
+      <c r="D6" s="385"/>
+      <c r="E6" s="385"/>
+      <c r="F6" s="385"/>
+      <c r="G6" s="385"/>
+      <c r="H6" s="385"/>
+      <c r="I6" s="385"/>
+      <c r="J6" s="386"/>
       <c r="K6" s="78" t="s">
         <v>134</v>
       </c>
@@ -15742,12 +15742,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="380" t="s">
+      <c r="K23" s="387" t="s">
         <v>107</v>
       </c>
-      <c r="L23" s="380"/>
-      <c r="M23" s="380"/>
-      <c r="N23" s="380"/>
+      <c r="L23" s="387"/>
+      <c r="M23" s="387"/>
+      <c r="N23" s="387"/>
       <c r="O23" s="35" t="s">
         <v>145</v>
       </c>
@@ -15916,7 +15916,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="376" t="s">
+      <c r="I28" s="383" t="s">
         <v>252</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15966,7 +15966,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="376"/>
+      <c r="I29" s="383"/>
       <c r="J29" s="82" t="s">
         <v>142</v>
       </c>
@@ -16014,7 +16014,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="376"/>
+      <c r="I30" s="383"/>
       <c r="J30" s="82" t="s">
         <v>141</v>
       </c>
@@ -16062,7 +16062,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="376"/>
+      <c r="I31" s="383"/>
       <c r="J31" s="35" t="s">
         <v>139</v>
       </c>
@@ -16124,7 +16124,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="376" t="s">
+      <c r="I33" s="383" t="s">
         <v>140</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -16172,7 +16172,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="376"/>
+      <c r="I34" s="383"/>
       <c r="J34" t="s">
         <v>253</v>
       </c>
@@ -16409,12 +16409,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -16422,6 +16416,12 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16528,22 +16528,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="389" t="s">
+      <c r="E6" s="391" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="389"/>
-      <c r="G6" s="389"/>
-      <c r="H6" s="389"/>
-      <c r="I6" s="389"/>
-      <c r="J6" s="389"/>
-      <c r="K6" s="389"/>
-      <c r="L6" s="389"/>
-      <c r="M6" s="389"/>
-      <c r="N6" s="389"/>
-      <c r="O6" s="389"/>
-      <c r="P6" s="389"/>
-      <c r="Q6" s="389"/>
-      <c r="R6" s="389"/>
+      <c r="F6" s="391"/>
+      <c r="G6" s="391"/>
+      <c r="H6" s="391"/>
+      <c r="I6" s="391"/>
+      <c r="J6" s="391"/>
+      <c r="K6" s="391"/>
+      <c r="L6" s="391"/>
+      <c r="M6" s="391"/>
+      <c r="N6" s="391"/>
+      <c r="O6" s="391"/>
+      <c r="P6" s="391"/>
+      <c r="Q6" s="391"/>
+      <c r="R6" s="391"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="388" t="s">
@@ -17279,21 +17279,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="390" t="s">
+      <c r="H27" s="389" t="s">
         <v>94</v>
       </c>
-      <c r="I27" s="390"/>
-      <c r="J27" s="390"/>
-      <c r="K27" s="390"/>
-      <c r="L27" s="390"/>
-      <c r="M27" s="390"/>
-      <c r="N27" s="390"/>
-      <c r="O27" s="390"/>
-      <c r="P27" s="390"/>
-      <c r="Q27" s="390"/>
-      <c r="R27" s="390"/>
-      <c r="S27" s="390"/>
-      <c r="T27" s="390"/>
+      <c r="I27" s="389"/>
+      <c r="J27" s="389"/>
+      <c r="K27" s="389"/>
+      <c r="L27" s="389"/>
+      <c r="M27" s="389"/>
+      <c r="N27" s="389"/>
+      <c r="O27" s="389"/>
+      <c r="P27" s="389"/>
+      <c r="Q27" s="389"/>
+      <c r="R27" s="389"/>
+      <c r="S27" s="389"/>
+      <c r="T27" s="389"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -17609,21 +17609,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="391" t="s">
+      <c r="F37" s="390" t="s">
         <v>98</v>
       </c>
-      <c r="G37" s="391"/>
-      <c r="H37" s="391"/>
-      <c r="I37" s="391"/>
-      <c r="J37" s="391"/>
-      <c r="K37" s="391"/>
-      <c r="L37" s="391"/>
-      <c r="M37" s="391"/>
-      <c r="N37" s="391"/>
-      <c r="O37" s="391"/>
-      <c r="P37" s="391"/>
-      <c r="Q37" s="391"/>
-      <c r="R37" s="391"/>
+      <c r="G37" s="390"/>
+      <c r="H37" s="390"/>
+      <c r="I37" s="390"/>
+      <c r="J37" s="390"/>
+      <c r="K37" s="390"/>
+      <c r="L37" s="390"/>
+      <c r="M37" s="390"/>
+      <c r="N37" s="390"/>
+      <c r="O37" s="390"/>
+      <c r="P37" s="390"/>
+      <c r="Q37" s="390"/>
+      <c r="R37" s="390"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -17939,21 +17939,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="390" t="s">
+      <c r="F48" s="389" t="s">
         <v>100</v>
       </c>
-      <c r="G48" s="390"/>
-      <c r="H48" s="390"/>
-      <c r="I48" s="390"/>
-      <c r="J48" s="390"/>
-      <c r="K48" s="390"/>
-      <c r="L48" s="390"/>
-      <c r="M48" s="390"/>
-      <c r="N48" s="390"/>
-      <c r="O48" s="390"/>
-      <c r="P48" s="390"/>
-      <c r="Q48" s="390"/>
-      <c r="R48" s="390"/>
+      <c r="G48" s="389"/>
+      <c r="H48" s="389"/>
+      <c r="I48" s="389"/>
+      <c r="J48" s="389"/>
+      <c r="K48" s="389"/>
+      <c r="L48" s="389"/>
+      <c r="M48" s="389"/>
+      <c r="N48" s="389"/>
+      <c r="O48" s="389"/>
+      <c r="P48" s="389"/>
+      <c r="Q48" s="389"/>
+      <c r="R48" s="389"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -18265,6 +18265,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -18273,12 +18279,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22524,13 +22524,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F6A688-71E8-4308-9AE6-7C668128D989}">
-  <dimension ref="A1:AW73"/>
+  <dimension ref="A1:AX73"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
+      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22548,7 +22548,7 @@
     <col min="27" max="27" width="8.6640625" style="146"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="360" t="s">
         <v>203</v>
       </c>
@@ -22564,7 +22564,7 @@
       <c r="X1" s="352"/>
       <c r="Y1" s="352"/>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="362" t="s">
         <v>189</v>
       </c>
@@ -22575,7 +22575,7 @@
       <c r="I2" s="241"/>
       <c r="J2" s="368"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="363"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
@@ -22584,21 +22584,21 @@
       <c r="I3" s="241"/>
       <c r="J3" s="368"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="363"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" s="364"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="C7" s="365" t="s">
         <v>159</v>
       </c>
@@ -22639,7 +22639,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>197</v>
       </c>
@@ -22719,7 +22719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:49" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="106" t="s">
         <v>162</v>
       </c>
@@ -22741,1151 +22741,1175 @@
       <c r="W9" s="148"/>
       <c r="AA9" s="148"/>
     </row>
-    <row r="10" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="86" t="s">
         <v>168</v>
       </c>
       <c r="D10">
+        <v>200.67099999999999</v>
+      </c>
+      <c r="E10">
         <v>156.16</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>197.62799999999999</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>170.20699999999999</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>164.137</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>168.283382790221</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>172.42976558044199</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>173.014858331521</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>173.599951082601</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>174.18504383368</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>174.77013658476</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>172.87701948733101</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>170.983902389902</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>169.09078529247299</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>167.197668195044</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>168.18650468764599</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>169.17534118024699</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>170.16417767284801</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>171.15301416545</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>173.69648926200901</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>176.23996435856799</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>178.783439455127</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>181.326914551686</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>183.85985203006999</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>186.392789508455</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>188.92572698683901</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>191.45866446522299</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>194.36254309952099</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>197.26642173381799</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>200.17030036811499</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>203.07417900241299</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>206.00159731602</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <v>208.929015629627</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>211.856433943235</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>214.78385225684201</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>217.808743538567</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>220.833634820291</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>223.85852610201599</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <v>226.883417383741</v>
       </c>
-      <c r="AP10">
+      <c r="AQ10">
         <v>230.07495599805301</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <v>233.26649461236599</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <v>236.458033226678</v>
       </c>
-      <c r="AS10">
+      <c r="AT10">
         <v>239.649571840991</v>
       </c>
-      <c r="AT10">
+      <c r="AU10">
         <v>242.96586225756701</v>
       </c>
-      <c r="AU10">
+      <c r="AV10">
         <v>246.28215267414299</v>
       </c>
-      <c r="AV10">
+      <c r="AW10">
         <v>249.598443090719</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <v>252.91473350729501</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="86" t="s">
         <v>169</v>
       </c>
       <c r="D11">
-        <v>440</v>
+        <v>143</v>
       </c>
       <c r="E11">
-        <v>363.8</v>
+        <v>143.4</v>
       </c>
       <c r="F11">
-        <v>243.1</v>
+        <v>144.80000000000001</v>
       </c>
       <c r="G11">
-        <v>216.8</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="H11">
-        <v>221.238806677822</v>
+        <v>145.9</v>
       </c>
       <c r="I11">
-        <v>221.863490042297</v>
+        <v>148.62914612772201</v>
       </c>
       <c r="J11">
-        <v>234.39138633050499</v>
+        <v>147.84327450886599</v>
       </c>
       <c r="K11">
-        <v>247.15695601015699</v>
+        <v>159.196596921229</v>
       </c>
       <c r="L11">
-        <v>260.16397055036401</v>
+        <v>170.768954252019</v>
       </c>
       <c r="M11">
-        <v>272.23431764689798</v>
+        <v>182.563822209747</v>
       </c>
       <c r="N11">
-        <v>293.691342591298</v>
+        <v>193.49547667995401</v>
       </c>
       <c r="O11">
-        <v>314.10658648539999</v>
+        <v>213.89148204176601</v>
       </c>
       <c r="P11">
-        <v>334.67508713304699</v>
+        <v>233.327403374037</v>
       </c>
       <c r="Q11">
-        <v>355.23230513680301</v>
+        <v>252.90456298421299</v>
       </c>
       <c r="R11">
-        <v>364.17283208422799</v>
+        <v>272.47132474139602</v>
       </c>
       <c r="S11">
-        <v>373.56443272323401</v>
+        <v>280.38602200487202</v>
       </c>
       <c r="T11">
-        <v>383.36610035458602</v>
+        <v>288.71641952254998</v>
       </c>
       <c r="U11">
-        <v>392.59367419665398</v>
+        <v>297.42472636223198</v>
       </c>
       <c r="V11">
-        <v>394.69632275445201</v>
+        <v>305.60396015110899</v>
       </c>
       <c r="W11">
-        <v>396.75796461301599</v>
+        <v>306.70650516123197</v>
       </c>
       <c r="X11">
-        <v>398.77859977234499</v>
+        <v>307.77125923915401</v>
       </c>
       <c r="Y11">
-        <v>400.79923493167399</v>
+        <v>308.79822238487702</v>
       </c>
       <c r="Z11">
-        <v>402.863994846369</v>
+        <v>309.82518553059901</v>
       </c>
       <c r="AA11">
-        <v>404.928754761064</v>
+        <v>310.89627343168797</v>
       </c>
       <c r="AB11">
-        <v>407.03452137499397</v>
+        <v>311.96736133277602</v>
       </c>
       <c r="AC11">
-        <v>409.140287988924</v>
+        <v>313.07624016606502</v>
       </c>
       <c r="AD11">
-        <v>409.73379874423102</v>
+        <v>314.18511899935402</v>
       </c>
       <c r="AE11">
-        <v>410.32730949953702</v>
+        <v>313.77852620698599</v>
       </c>
       <c r="AF11">
-        <v>410.96182695407902</v>
+        <v>313.37193341461699</v>
       </c>
       <c r="AG11">
-        <v>411.63735110785501</v>
+        <v>313.003131554449</v>
       </c>
       <c r="AH11">
-        <v>412.21430625165902</v>
+        <v>312.67212062648099</v>
       </c>
       <c r="AI11">
-        <v>412.79126139546298</v>
+        <v>312.242540688541</v>
       </c>
       <c r="AJ11">
-        <v>413.40922323850202</v>
+        <v>311.81296075060101</v>
       </c>
       <c r="AK11">
-        <v>414.02718508154101</v>
+        <v>311.42117174486202</v>
       </c>
       <c r="AL11">
-        <v>414.27799963667502</v>
+        <v>311.02938273912201</v>
       </c>
       <c r="AM11">
-        <v>414.52881419180898</v>
+        <v>310.26723067844398</v>
       </c>
       <c r="AN11">
-        <v>414.77962874694299</v>
+        <v>309.505078617766</v>
       </c>
       <c r="AO11">
-        <v>415.07145000131197</v>
+        <v>308.742926557087</v>
       </c>
       <c r="AP11">
-        <v>414.74747299871802</v>
+        <v>308.01856542860901</v>
       </c>
       <c r="AQ11">
-        <v>414.46450269535899</v>
+        <v>306.67197450909902</v>
       </c>
       <c r="AR11">
-        <v>414.26354579046898</v>
+        <v>305.363174521791</v>
       </c>
       <c r="AS11">
-        <v>414.14460228404897</v>
+        <v>304.12995639888197</v>
       </c>
       <c r="AT11">
-        <v>413.58529200772699</v>
+        <v>302.97232014037399</v>
       </c>
       <c r="AU11">
-        <v>413.10799512987501</v>
+        <v>301.36788557789703</v>
       </c>
       <c r="AV11">
-        <v>412.753718349726</v>
+        <v>299.83903287982002</v>
       </c>
       <c r="AW11">
-        <v>412.44044826881299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+        <v>298.42355297834399</v>
+      </c>
+      <c r="AX11">
+        <v>297.04586400906902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="86" t="s">
         <v>170</v>
       </c>
       <c r="D12">
+        <v>1862.4</v>
+      </c>
+      <c r="E12">
         <v>1779.8</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1871.3</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1907.1</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1958.3</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1978.3751090344099</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2007.0179878174299</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2033.6981662082601</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2058.9444082394798</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>2079.7902580671698</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>2102.1686273791902</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>2124.25124731704</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2144.5772952143798</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2167.3231107185502</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2191.2429616171398</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>2215.89770490003</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>2239.1633223345498</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>2263.8359898219301</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>2288.6968614565099</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>2314.5704506450502</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>2339.87046528976</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>2365.3049114681799</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>2390.1837073072502</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>2414.9370337148598</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>2439.8964884741599</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>2464.3361413031098</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>2488.5158931668698</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>2512.2565020205102</v>
       </c>
-      <c r="AE12">
+      <c r="AF12">
         <v>2535.6655130909999</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>2559.0834862637298</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>2582.8330572196101</v>
       </c>
-      <c r="AH12">
+      <c r="AI12">
         <v>2607.0934680036098</v>
       </c>
-      <c r="AI12">
+      <c r="AJ12">
         <v>2631.7661354909901</v>
       </c>
-      <c r="AJ12">
+      <c r="AK12">
         <v>2656.7704007615298</v>
       </c>
-      <c r="AK12">
+      <c r="AL12">
         <v>2681.7298555208299</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>2706.7878934048499</v>
       </c>
-      <c r="AM12">
+      <c r="AN12">
         <v>2731.9265902091001</v>
       </c>
-      <c r="AN12">
+      <c r="AO12">
         <v>2757.0204765021099</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>2782.0157796704102</v>
       </c>
-      <c r="AP12">
+      <c r="AQ12">
         <v>2807.24409749713</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>2832.5441121418398</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>2858.14883826296</v>
       </c>
-      <c r="AS12">
+      <c r="AT12">
         <v>2884.24648000769</v>
       </c>
-      <c r="AT12">
+      <c r="AU12">
         <v>2910.8011889670502</v>
       </c>
-      <c r="AU12">
+      <c r="AV12">
         <v>2937.8756998567601</v>
       </c>
-      <c r="AV12">
+      <c r="AW12">
         <v>2965.0487938711899</v>
       </c>
-      <c r="AW12">
+      <c r="AX12">
         <v>2992.3742436238399</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="86" t="s">
         <v>171</v>
       </c>
       <c r="D13">
+        <v>62.7</v>
+      </c>
+      <c r="E13">
         <v>54.2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>90.2</v>
-      </c>
-      <c r="F13">
-        <v>95.9</v>
       </c>
       <c r="G13">
         <v>95.9</v>
       </c>
       <c r="H13">
+        <v>95.9</v>
+      </c>
+      <c r="I13">
         <v>96.883099094316506</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>98.285770837814496</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>99.592327089502007</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>100.82866197731001</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>101.849505054712</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>102.94539721476001</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>104.026806218508</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>105.022194051504</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>106.136080436046</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>107.30746056226501</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>108.514829137473</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>109.654170766422</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>110.86241710867699</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>112.07988000494301</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>113.346936739448</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>114.58590492840101</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>115.83145637021801</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>117.049797033532</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>118.261993327506</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>119.484283942538</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>120.68111931316299</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>121.865227061586</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>123.02782951732</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>124.174193282657</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>125.320995931518</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>126.484037270776</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>127.672094970917</v>
       </c>
-      <c r="AI13">
+      <c r="AJ13">
         <v>128.88034131317301</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>130.10482634582601</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>131.32711696085801</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>132.554235294656</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>133.78530358017301</v>
       </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>135.01417744806901</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
         <v>136.23822359719799</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>137.473680717957</v>
       </c>
-      <c r="AQ13">
+      <c r="AR13">
         <v>138.71264890691</v>
       </c>
-      <c r="AR13">
+      <c r="AS13">
         <v>139.96653913568801</v>
       </c>
-      <c r="AS13">
+      <c r="AT13">
         <v>141.244567958299</v>
       </c>
-      <c r="AT13">
+      <c r="AU13">
         <v>142.54497984064699</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>143.870846967402</v>
       </c>
-      <c r="AV13">
+      <c r="AW13">
         <v>145.20154181292301</v>
       </c>
-      <c r="AW13">
+      <c r="AX13">
         <v>146.53969767835699</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="86" t="s">
         <v>173</v>
       </c>
       <c r="D14">
+        <v>1228.1289999999999</v>
+      </c>
+      <c r="E14">
         <v>1336.74</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1328.7719999999999</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1372.7929999999999</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1403.2629999999999</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>1394.63952711825</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1386.0160542364999</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1416.24742986613</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>1446.4788054957501</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>1476.7101811253699</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>1506.941556755</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>1519.7601557667999</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>1532.5787547785901</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>1545.3973537903901</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>1558.21595280219</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1568.7825477363999</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>1579.34914267061</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>1589.9157376048099</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>1600.48233253902</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>1639.9186754518</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>1679.35501836459</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>1718.79136127737</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>1758.22770419015</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>1787.6196955994999</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>1817.01168700885</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>1846.4036784181901</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>1875.79566982754</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>1908.2148727936301</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>1940.63407575972</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>1973.0532787258101</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>2005.4724816918999</v>
       </c>
-      <c r="AH14">
+      <c r="AI14">
         <v>2057.1759873287501</v>
       </c>
-      <c r="AI14">
+      <c r="AJ14">
         <v>2108.8794929656101</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>2160.5829986024601</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>2212.28650423931</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>2211.5343138466101</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>2210.7821234539101</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>2210.0299330612002</v>
       </c>
-      <c r="AO14">
+      <c r="AP14">
         <v>2209.2777426685002</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>2261.6493087725698</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>2314.0208748766299</v>
       </c>
-      <c r="AR14">
+      <c r="AS14">
         <v>2366.3924409807</v>
       </c>
-      <c r="AS14">
+      <c r="AT14">
         <v>2418.7640070847701</v>
       </c>
-      <c r="AT14">
+      <c r="AU14">
         <v>2464.36520513099</v>
       </c>
-      <c r="AU14">
+      <c r="AV14">
         <v>2509.9664031771999</v>
       </c>
-      <c r="AV14">
+      <c r="AW14">
         <v>2555.5676012234098</v>
       </c>
-      <c r="AW14">
+      <c r="AX14">
         <v>2601.1687992696202</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="86" t="s">
         <v>164</v>
       </c>
       <c r="D15">
+        <v>1574.4</v>
+      </c>
+      <c r="E15">
         <v>1828.5</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1861.4</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1756.2</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>1808.7</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1629.3563571043301</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1501.6652887165701</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1514.2729452476999</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1515.61502429495</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1509.9264163187599</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>1493.71783405563</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>1512.9609535468801</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>1522.99399388232</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>1526.52581787499</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>1522.58327322214</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>1530.28560256998</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>1538.9373350641299</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>1547.1929515766401</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>1555.9808389633299</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>1592.1555871790999</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>1622.7235946783901</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>1646.251758186</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>1663.41962105019</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>1671.4306991660901</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>1682.1431104472799</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>1694.6607802102701</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>1709.3896382183</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>1722.3726155766301</v>
       </c>
-      <c r="AE15">
+      <c r="AF15">
         <v>1735.04294744297</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>1746.49533930811</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>1757.18821215652</v>
       </c>
-      <c r="AH15">
+      <c r="AI15">
         <v>1788.9509959744801</v>
       </c>
-      <c r="AI15">
+      <c r="AJ15">
         <v>1816.7189541257301</v>
       </c>
-      <c r="AJ15">
+      <c r="AK15">
         <v>1839.6922791597999</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>1858.25973323063</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>1832.42941895323</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>1818.5767493211199</v>
       </c>
-      <c r="AN15">
+      <c r="AO15">
         <v>1816.44046526276</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <v>1826.1076220744501</v>
       </c>
-      <c r="AP15">
+      <c r="AQ15">
         <v>1883.5218401063901</v>
       </c>
-      <c r="AQ15">
+      <c r="AR15">
         <v>1928.4971849546901</v>
       </c>
-      <c r="AR15">
+      <c r="AS15">
         <v>1962.1388593722199</v>
       </c>
-      <c r="AS15">
+      <c r="AT15">
         <v>1983.8010497242601</v>
       </c>
-      <c r="AT15">
+      <c r="AU15">
         <v>1944.7885028241201</v>
       </c>
-      <c r="AU15">
+      <c r="AV15">
         <v>1906.4485972733501</v>
       </c>
-      <c r="AV15">
+      <c r="AW15">
         <v>1870.23933365998</v>
       </c>
-      <c r="AW15">
+      <c r="AX15">
         <v>1835.4218257479599</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="86" t="s">
         <v>167</v>
       </c>
       <c r="D16">
+        <v>74.5</v>
+      </c>
+      <c r="E16">
         <v>1085.9000000000001</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1212.9000000000001</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>609.79999999999995</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>402.3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>404.18538158623397</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>406.11408156777497</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>408.08197438316603</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>410.07255778657401</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>412.05076450561</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>413.998029513711</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>415.93291783743899</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>417.86368059970903</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>419.80063170416599</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>421.75614783518301</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>423.73022899275998</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>425.71668683471103</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>427.69901911520401</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>429.68753973788398</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>431.68018592202202</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>433.67076932543</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>435.63659936009202</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>437.58798992965097</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>439.524941034108</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>441.44951545419099</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>443.35552484771398</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>445.259471460508</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>447.16548085403099</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>449.07355302828302</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>450.98368798326402</v>
       </c>
-      <c r="AG16">
+      <c r="AH16">
         <v>452.90619962261798</v>
       </c>
-      <c r="AH16">
+      <c r="AI16">
         <v>454.83283682343102</v>
       </c>
-      <c r="AI16">
+      <c r="AJ16">
         <v>456.76772514715901</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>458.72736683963302</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>460.70763633939799</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>462.71059642718001</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <v>464.73212154152202</v>
       </c>
-      <c r="AN16">
+      <c r="AO16">
         <v>466.76808612096698</v>
       </c>
-      <c r="AO16">
+      <c r="AP16">
         <v>468.801987919684</v>
       </c>
-      <c r="AP16">
+      <c r="AQ16">
         <v>470.83176415694197</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>472.86360317492898</v>
       </c>
-      <c r="AR16">
+      <c r="AS16">
         <v>474.89544219291599</v>
       </c>
-      <c r="AS16">
+      <c r="AT16">
         <v>476.927281210903</v>
       </c>
-      <c r="AT16">
+      <c r="AU16">
         <v>478.965308571077</v>
       </c>
-      <c r="AU16">
+      <c r="AV16">
         <v>481.00539871197998</v>
       </c>
-      <c r="AV16">
+      <c r="AW16">
         <v>483.04961441434102</v>
       </c>
-      <c r="AW16">
+      <c r="AX16">
         <v>485.09176733597201</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>193</v>
       </c>
       <c r="D17">
+        <v>204.37100000000001</v>
+      </c>
+      <c r="E17">
         <v>884.26</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>242.12799999999999</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>225.90700000000001</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>260.73700000000002</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>255.59948840017799</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>254.55541346215</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>256.89572380491899</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>259.47104592492298</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>261.94028245643398</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>264.42386516359801</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>266.96509198785299</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>269.50680093709798</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>272.09622896230098</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>274.73279727509299</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>277.43299355096599</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>280.18660377739002</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>282.96027933542803</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>285.76787991439801</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>288.60599468885499</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>291.45669283695003</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>294.32349490703803</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>297.203923810513</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>300.10743213158901</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>303.03076239752602</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>305.96732781542198</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>308.933269814786</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>311.92682031928803</v>
       </c>
-      <c r="AE17">
+      <c r="AF17">
         <v>314.95057777842101</v>
       </c>
-      <c r="AF17">
+      <c r="AG17">
         <v>317.99988617750199</v>
       </c>
-      <c r="AG17">
+      <c r="AH17">
         <v>321.08460698104102</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <v>324.19918656622298</v>
       </c>
-      <c r="AI17">
+      <c r="AJ17">
         <v>327.32952746436501</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>330.49490821139301</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>333.69267244823402</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>336.92458346914202</v>
       </c>
-      <c r="AM17">
+      <c r="AN17">
         <v>340.18041466745098</v>
       </c>
-      <c r="AN17">
+      <c r="AO17">
         <v>343.46484362914902</v>
       </c>
-      <c r="AO17">
+      <c r="AP17">
         <v>346.76592631979901</v>
       </c>
-      <c r="AP17">
+      <c r="AQ17">
         <v>350.08468421354098</v>
       </c>
-      <c r="AQ17">
+      <c r="AR17">
         <v>353.42318738029297</v>
       </c>
-      <c r="AR17">
+      <c r="AS17">
         <v>356.77995072225002</v>
       </c>
-      <c r="AS17">
+      <c r="AT17">
         <v>360.15500702948498</v>
       </c>
-      <c r="AT17">
+      <c r="AU17">
         <v>363.555644240942</v>
       </c>
-      <c r="AU17">
+      <c r="AV17">
         <v>366.97627559402702</v>
       </c>
-      <c r="AV17">
+      <c r="AW17">
         <v>370.42373968929098</v>
       </c>
-      <c r="AW17">
+      <c r="AX17">
         <v>373.88820823868502</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
       <c r="E19" s="95"/>
       <c r="F19" s="95"/>
       <c r="L19" s="95"/>
@@ -23902,7 +23926,7 @@
       <c r="Z19" s="95"/>
       <c r="AB19" s="95"/>
     </row>
-    <row r="20" spans="1:49" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="110" t="s">
         <v>182</v>
       </c>
@@ -23923,7 +23947,7 @@
       <c r="Z20" s="95"/>
       <c r="AB20" s="95"/>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>182</v>
       </c>
@@ -24022,7 +24046,7 @@
       </c>
       <c r="AB21" s="95"/>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>175</v>
       </c>
@@ -24031,14 +24055,14 @@
         <v>#REF!</v>
       </c>
       <c r="E22" s="104">
-        <f t="shared" ref="E22:AA22" si="1">D10</f>
+        <f>E10</f>
         <v>156.16</v>
       </c>
       <c r="F22" s="104">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F22:AA22" si="1">F10</f>
         <v>197.62799999999999</v>
       </c>
-      <c r="G22" s="149">
+      <c r="G22" s="104">
         <f t="shared" si="1"/>
         <v>170.20699999999999</v>
       </c>
@@ -24054,7 +24078,7 @@
         <f t="shared" si="1"/>
         <v>172.42976558044199</v>
       </c>
-      <c r="K22" s="149">
+      <c r="K22" s="104">
         <f t="shared" si="1"/>
         <v>173.014858331521</v>
       </c>
@@ -24062,7 +24086,7 @@
         <f t="shared" si="1"/>
         <v>173.599951082601</v>
       </c>
-      <c r="M22" s="223">
+      <c r="M22" s="104">
         <f t="shared" si="1"/>
         <v>174.18504383368</v>
       </c>
@@ -24070,7 +24094,7 @@
         <f t="shared" si="1"/>
         <v>174.77013658476</v>
       </c>
-      <c r="O22" s="149">
+      <c r="O22" s="104">
         <f t="shared" si="1"/>
         <v>172.87701948733101</v>
       </c>
@@ -24086,7 +24110,7 @@
         <f t="shared" si="1"/>
         <v>167.197668195044</v>
       </c>
-      <c r="S22" s="149">
+      <c r="S22" s="104">
         <f t="shared" si="1"/>
         <v>168.18650468764599</v>
       </c>
@@ -24102,7 +24126,7 @@
         <f t="shared" si="1"/>
         <v>171.15301416545</v>
       </c>
-      <c r="W22" s="149">
+      <c r="W22" s="104">
         <f t="shared" si="1"/>
         <v>173.69648926200901</v>
       </c>
@@ -24118,13 +24142,13 @@
         <f t="shared" si="1"/>
         <v>181.326914551686</v>
       </c>
-      <c r="AA22" s="149">
+      <c r="AA22" s="104">
         <f t="shared" si="1"/>
         <v>183.85985203006999</v>
       </c>
       <c r="AB22" s="95"/>
     </row>
-    <row r="23" spans="1:49" s="170" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:50" s="170" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="B23" s="210" t="s">
         <v>271</v>
       </c>
@@ -24196,7 +24220,7 @@
       </c>
       <c r="AB23" s="243"/>
     </row>
-    <row r="24" spans="1:49" s="97" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" s="97" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="99" t="s">
         <v>176</v>
       </c>
@@ -24292,7 +24316,7 @@
       </c>
       <c r="AB24" s="244"/>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
       <c r="D25" s="102"/>
       <c r="E25" s="104"/>
       <c r="F25" s="104"/>
@@ -24315,7 +24339,7 @@
       <c r="Z25" s="95"/>
       <c r="AB25" s="95"/>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="D26" s="102"/>
       <c r="E26" s="104"/>
       <c r="F26" s="104"/>
@@ -24338,7 +24362,7 @@
       <c r="Z26" s="95"/>
       <c r="AB26" s="95"/>
     </row>
-    <row r="27" spans="1:49" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="110" t="s">
         <v>185</v>
       </c>
@@ -24365,7 +24389,7 @@
       <c r="Z27" s="95"/>
       <c r="AB27" s="95"/>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>185</v>
       </c>
@@ -24404,67 +24428,67 @@
       </c>
       <c r="M28" s="104">
         <f>L28*(1 + M30)</f>
-        <v>203.30373636403701</v>
+        <v>206.47945574985528</v>
       </c>
       <c r="N28" s="104">
         <f t="shared" ref="N28:AA28" si="22">M28*(1 + N30)</f>
-        <v>212.73604422259618</v>
+        <v>218.84314335309011</v>
       </c>
       <c r="O28" s="104">
         <f t="shared" si="22"/>
-        <v>229.50352103049028</v>
+        <v>241.91100003796859</v>
       </c>
       <c r="P28" s="104">
         <f t="shared" si="22"/>
-        <v>245.45690363636709</v>
+        <v>263.89300288009605</v>
       </c>
       <c r="Q28" s="104">
         <f t="shared" si="22"/>
-        <v>261.53004790852236</v>
+        <v>286.03474603878726</v>
       </c>
       <c r="R28" s="104">
         <f t="shared" si="22"/>
-        <v>277.59437541925496</v>
+        <v>308.16472923868179</v>
       </c>
       <c r="S28" s="104">
         <f t="shared" si="22"/>
-        <v>284.58090214557194</v>
+        <v>317.11624199518968</v>
       </c>
       <c r="T28" s="104">
         <f t="shared" si="22"/>
-        <v>291.91991798358237</v>
+        <v>326.53791122193229</v>
       </c>
       <c r="U28" s="104">
         <f t="shared" si="22"/>
-        <v>299.57937846858658</v>
+        <v>336.38699542161817</v>
       </c>
       <c r="V28" s="104">
         <f t="shared" si="22"/>
-        <v>306.79021644779976</v>
+        <v>345.63769865918431</v>
       </c>
       <c r="W28" s="104">
         <f t="shared" si="22"/>
-        <v>308.433319861222</v>
+        <v>346.88467569370516</v>
       </c>
       <c r="X28" s="104">
         <f t="shared" si="22"/>
-        <v>310.04437880994533</v>
+        <v>348.0889112309311</v>
       </c>
       <c r="Y28" s="104">
         <f t="shared" si="22"/>
-        <v>311.623393293969</v>
+        <v>349.25040527086435</v>
       </c>
       <c r="Z28" s="104">
         <f t="shared" si="22"/>
-        <v>313.20240777799268</v>
+        <v>350.4118993107964</v>
       </c>
       <c r="AA28" s="104">
         <f t="shared" si="22"/>
-        <v>314.81590331491952</v>
+        <v>351.62329839414281</v>
       </c>
       <c r="AB28" s="95"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>175</v>
       </c>
@@ -24473,100 +24497,100 @@
         <v>#REF!</v>
       </c>
       <c r="E29" s="104">
-        <f t="shared" ref="E29:AA29" si="23">D11</f>
-        <v>440</v>
+        <f>E11</f>
+        <v>143.4</v>
       </c>
       <c r="F29" s="104">
+        <f t="shared" ref="F29:U30" si="23">F11</f>
+        <v>144.80000000000001</v>
+      </c>
+      <c r="G29" s="104">
         <f t="shared" si="23"/>
-        <v>363.8</v>
-      </c>
-      <c r="G29" s="149">
-        <f t="shared" si="23"/>
-        <v>243.1</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="H29" s="104">
         <f t="shared" si="23"/>
-        <v>216.8</v>
+        <v>145.9</v>
       </c>
       <c r="I29" s="104">
         <f t="shared" si="23"/>
-        <v>221.238806677822</v>
+        <v>148.62914612772201</v>
       </c>
       <c r="J29" s="104">
         <f t="shared" si="23"/>
-        <v>221.863490042297</v>
-      </c>
-      <c r="K29" s="149">
+        <v>147.84327450886599</v>
+      </c>
+      <c r="K29" s="104">
         <f t="shared" si="23"/>
-        <v>234.39138633050499</v>
-      </c>
-      <c r="L29" s="223">
+        <v>159.196596921229</v>
+      </c>
+      <c r="L29" s="104">
         <f t="shared" si="23"/>
-        <v>247.15695601015699</v>
+        <v>170.768954252019</v>
       </c>
       <c r="M29" s="104">
         <f t="shared" si="23"/>
-        <v>260.16397055036401</v>
+        <v>182.563822209747</v>
       </c>
       <c r="N29" s="104">
         <f t="shared" si="23"/>
-        <v>272.23431764689798</v>
-      </c>
-      <c r="O29" s="149">
+        <v>193.49547667995401</v>
+      </c>
+      <c r="O29" s="104">
         <f t="shared" si="23"/>
-        <v>293.691342591298</v>
+        <v>213.89148204176601</v>
       </c>
       <c r="P29" s="104">
         <f t="shared" si="23"/>
-        <v>314.10658648539999</v>
+        <v>233.327403374037</v>
       </c>
       <c r="Q29" s="104">
         <f t="shared" si="23"/>
-        <v>334.67508713304699</v>
+        <v>252.90456298421299</v>
       </c>
       <c r="R29" s="104">
         <f t="shared" si="23"/>
-        <v>355.23230513680301</v>
-      </c>
-      <c r="S29" s="149">
+        <v>272.47132474139602</v>
+      </c>
+      <c r="S29" s="104">
         <f t="shared" si="23"/>
-        <v>364.17283208422799</v>
+        <v>280.38602200487202</v>
       </c>
       <c r="T29" s="104">
         <f t="shared" si="23"/>
-        <v>373.56443272323401</v>
+        <v>288.71641952254998</v>
       </c>
       <c r="U29" s="104">
         <f t="shared" si="23"/>
-        <v>383.36610035458602</v>
+        <v>297.42472636223198</v>
       </c>
       <c r="V29" s="104">
-        <f t="shared" si="23"/>
-        <v>392.59367419665398</v>
-      </c>
-      <c r="W29" s="149">
-        <f t="shared" si="23"/>
-        <v>394.69632275445201</v>
+        <f t="shared" ref="V29:AA29" si="24">V11</f>
+        <v>305.60396015110899</v>
+      </c>
+      <c r="W29" s="104">
+        <f t="shared" si="24"/>
+        <v>306.70650516123197</v>
       </c>
       <c r="X29" s="104">
-        <f t="shared" si="23"/>
-        <v>396.75796461301599</v>
+        <f t="shared" si="24"/>
+        <v>307.77125923915401</v>
       </c>
       <c r="Y29" s="104">
-        <f t="shared" si="23"/>
-        <v>398.77859977234499</v>
+        <f t="shared" si="24"/>
+        <v>308.79822238487702</v>
       </c>
       <c r="Z29" s="104">
-        <f t="shared" si="23"/>
-        <v>400.79923493167399</v>
-      </c>
-      <c r="AA29" s="149">
-        <f t="shared" si="23"/>
-        <v>402.863994846369</v>
+        <f t="shared" si="24"/>
+        <v>309.82518553059901</v>
+      </c>
+      <c r="AA29" s="104">
+        <f t="shared" si="24"/>
+        <v>310.89627343168797</v>
       </c>
       <c r="AB29" s="95"/>
     </row>
-    <row r="30" spans="1:49" s="170" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:50" s="170" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="B30" s="210" t="s">
         <v>271</v>
       </c>
@@ -24580,164 +24604,164 @@
       <c r="K30" s="246"/>
       <c r="L30" s="230"/>
       <c r="M30" s="230">
-        <f t="shared" ref="M30" si="24">(M29/L29)-1</f>
-        <v>5.2626536392819556E-2</v>
+        <f t="shared" ref="M30" si="25">(M29/L29)-1</f>
+        <v>6.9069158439192924E-2</v>
       </c>
       <c r="N30" s="230">
-        <f t="shared" ref="N30" si="25">(N29/M29)-1</f>
-        <v>4.6395152530151362E-2</v>
+        <f t="shared" ref="N30" si="26">(N29/M29)-1</f>
+        <v>5.9878536381910763E-2</v>
       </c>
       <c r="O30" s="246">
-        <f t="shared" ref="O30" si="26">(O29/N29)-1</f>
-        <v>7.8818222220722767E-2</v>
+        <f t="shared" ref="O30" si="27">(O29/N29)-1</f>
+        <v>0.10540817652056789</v>
       </c>
       <c r="P30" s="230">
-        <f t="shared" ref="P30" si="27">(P29/O29)-1</f>
-        <v>6.951258322419096E-2</v>
+        <f t="shared" ref="P30" si="28">(P29/O29)-1</f>
+        <v>9.0868140922394369E-2</v>
       </c>
       <c r="Q30" s="230">
-        <f t="shared" ref="Q30" si="28">(Q29/P29)-1</f>
-        <v>6.5482551250491072E-2</v>
+        <f t="shared" ref="Q30" si="29">(Q29/P29)-1</f>
+        <v>8.3904244966857444E-2</v>
       </c>
       <c r="R30" s="230">
-        <f t="shared" ref="R30" si="29">(R29/Q29)-1</f>
-        <v>6.1424404725959336E-2</v>
+        <f t="shared" ref="R30" si="30">(R29/Q29)-1</f>
+        <v>7.7368164205105394E-2</v>
       </c>
       <c r="S30" s="246">
-        <f t="shared" ref="S30" si="30">(S29/R29)-1</f>
-        <v>2.5168113423642335E-2</v>
+        <f t="shared" ref="S30" si="31">(S29/R29)-1</f>
+        <v>2.9047817310639434E-2</v>
       </c>
       <c r="T30" s="230">
-        <f t="shared" ref="T30" si="31">(T29/S29)-1</f>
-        <v>2.5788855761853968E-2</v>
+        <f t="shared" ref="T30" si="32">(T29/S29)-1</f>
+        <v>2.9710459380650533E-2</v>
       </c>
       <c r="U30" s="230">
-        <f t="shared" ref="U30" si="32">(U29/T29)-1</f>
-        <v>2.6238224982767289E-2</v>
+        <f t="shared" ref="U30" si="33">(U29/T29)-1</f>
+        <v>3.0162146143551283E-2</v>
       </c>
       <c r="V30" s="230">
-        <f t="shared" ref="V30" si="33">(V29/U29)-1</f>
-        <v>2.4069874288658033E-2</v>
+        <f t="shared" ref="V30" si="34">(V29/U29)-1</f>
+        <v>2.7500180932891194E-2</v>
       </c>
       <c r="W30" s="246">
-        <f t="shared" ref="W30" si="34">(W29/V29)-1</f>
-        <v>5.3557881748873548E-3</v>
+        <f t="shared" ref="W30" si="35">(W29/V29)-1</f>
+        <v>3.607757600974093E-3</v>
       </c>
       <c r="X30" s="230">
-        <f t="shared" ref="X30" si="35">(X29/W29)-1</f>
-        <v>5.2233622147186409E-3</v>
+        <f t="shared" ref="X30" si="36">(X29/W29)-1</f>
+        <v>3.4715731815413431E-3</v>
       </c>
       <c r="Y30" s="230">
-        <f t="shared" ref="Y30" si="36">(Y29/X29)-1</f>
-        <v>5.0928660280327165E-3</v>
+        <f t="shared" ref="Y30" si="37">(Y29/X29)-1</f>
+        <v>3.3367740323180239E-3</v>
       </c>
       <c r="Z30" s="230">
-        <f t="shared" ref="Z30" si="37">(Z29/Y29)-1</f>
-        <v>5.0670601694338124E-3</v>
+        <f t="shared" ref="Z30" si="38">(Z29/Y29)-1</f>
+        <v>3.3256769996623525E-3</v>
       </c>
       <c r="AA30" s="246">
-        <f t="shared" ref="AA30" si="38">(AA29/Z29)-1</f>
-        <v>5.1516064272103534E-3</v>
+        <f t="shared" ref="AA30" si="39">(AA29/Z29)-1</f>
+        <v>3.4570717653397143E-3</v>
       </c>
       <c r="AB30" s="243"/>
     </row>
-    <row r="31" spans="1:49" s="97" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" s="97" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="99" t="s">
         <v>176</v>
       </c>
       <c r="D31" s="103"/>
       <c r="E31" s="217"/>
       <c r="F31" s="217">
-        <f t="shared" ref="F31" si="39">F28-F29</f>
-        <v>-33.023000000000025</v>
+        <f t="shared" ref="F31" si="40">F28-F29</f>
+        <v>185.97699999999998</v>
       </c>
       <c r="G31" s="150">
-        <f t="shared" ref="G31" si="40">G28-G29</f>
-        <v>-61.292000000000002</v>
+        <f t="shared" ref="G31" si="41">G28-G29</f>
+        <v>36.608000000000004</v>
       </c>
       <c r="H31" s="217">
-        <f t="shared" ref="H31" si="41">H28-H29</f>
-        <v>-10.88900000000001</v>
+        <f t="shared" ref="H31" si="42">H28-H29</f>
+        <v>60.010999999999996</v>
       </c>
       <c r="I31" s="217">
-        <f t="shared" ref="I31" si="42">I28-I29</f>
-        <v>-31.404359752822046</v>
+        <f t="shared" ref="I31" si="43">I28-I29</f>
+        <v>41.205300797277943</v>
       </c>
       <c r="J31" s="217">
-        <f t="shared" ref="J31" si="43">J28-J29</f>
-        <v>-31.299870882672082</v>
+        <f t="shared" ref="J31" si="44">J28-J29</f>
+        <v>42.720344650758932</v>
       </c>
       <c r="K31" s="150">
-        <f t="shared" ref="K31:N31" si="44">K28-K29</f>
-        <v>-42.728540027182873</v>
+        <f t="shared" ref="K31:N31" si="45">K28-K29</f>
+        <v>32.46624938209311</v>
       </c>
       <c r="L31" s="239">
-        <f t="shared" si="44"/>
-        <v>-54.017481243801626</v>
+        <f t="shared" si="45"/>
+        <v>22.370520514336363</v>
       </c>
       <c r="M31" s="217">
-        <f t="shared" si="44"/>
-        <v>-56.860234186327006</v>
+        <f t="shared" si="45"/>
+        <v>23.915633540108274</v>
       </c>
       <c r="N31" s="217">
-        <f t="shared" si="44"/>
-        <v>-59.4982734243018</v>
+        <f t="shared" si="45"/>
+        <v>25.347666673136104</v>
       </c>
       <c r="O31" s="150">
-        <f t="shared" ref="O31:AA31" si="45">O28-O29</f>
-        <v>-64.18782156080772</v>
+        <f t="shared" ref="O31:AA31" si="46">O28-O29</f>
+        <v>28.01951799620258</v>
       </c>
       <c r="P31" s="150">
-        <f t="shared" si="45"/>
-        <v>-68.649682849032899</v>
+        <f t="shared" si="46"/>
+        <v>30.565599506059044</v>
       </c>
       <c r="Q31" s="150">
-        <f t="shared" si="45"/>
-        <v>-73.145039224524623</v>
+        <f t="shared" si="46"/>
+        <v>33.130183054574275</v>
       </c>
       <c r="R31" s="150">
-        <f t="shared" si="45"/>
-        <v>-77.637929717548047</v>
+        <f t="shared" si="46"/>
+        <v>35.693404497285769</v>
       </c>
       <c r="S31" s="150">
-        <f t="shared" si="45"/>
-        <v>-79.591929938656051</v>
+        <f t="shared" si="46"/>
+        <v>36.730219990317664</v>
       </c>
       <c r="T31" s="150">
-        <f t="shared" si="45"/>
-        <v>-81.64451473965164</v>
+        <f t="shared" si="46"/>
+        <v>37.821491699382307</v>
       </c>
       <c r="U31" s="150">
-        <f t="shared" si="45"/>
-        <v>-83.786721885999441</v>
+        <f t="shared" si="46"/>
+        <v>38.962269059386188</v>
       </c>
       <c r="V31" s="150">
-        <f t="shared" si="45"/>
-        <v>-85.803457748854214</v>
+        <f t="shared" si="46"/>
+        <v>40.033738508075317</v>
       </c>
       <c r="W31" s="150">
-        <f t="shared" si="45"/>
-        <v>-86.263002893230009</v>
+        <f t="shared" si="46"/>
+        <v>40.178170532473189</v>
       </c>
       <c r="X31" s="150">
-        <f t="shared" si="45"/>
-        <v>-86.713585803070657</v>
+        <f t="shared" si="46"/>
+        <v>40.317651991777097</v>
       </c>
       <c r="Y31" s="150">
-        <f t="shared" si="45"/>
-        <v>-87.155206478375987</v>
+        <f t="shared" si="46"/>
+        <v>40.452182885987327</v>
       </c>
       <c r="Z31" s="150">
-        <f t="shared" si="45"/>
-        <v>-87.596827153681318</v>
+        <f t="shared" si="46"/>
+        <v>40.586713780197385</v>
       </c>
       <c r="AA31" s="150">
-        <f t="shared" si="45"/>
-        <v>-88.048091531449472</v>
+        <f t="shared" si="46"/>
+        <v>40.727024962454834</v>
       </c>
       <c r="AB31" s="244"/>
     </row>
-    <row r="32" spans="1:49" s="97" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" s="97" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="99"/>
       <c r="D32" s="103"/>
       <c r="E32" s="217"/>
@@ -24876,31 +24900,31 @@
         <v>#REF!</v>
       </c>
       <c r="E36" s="104">
-        <f t="shared" ref="E36:K36" si="46">D12</f>
+        <f>E12</f>
         <v>1779.8</v>
       </c>
       <c r="F36" s="104">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="F36:K36" si="47">F12</f>
         <v>1871.3</v>
       </c>
-      <c r="G36" s="149">
-        <f t="shared" si="46"/>
+      <c r="G36" s="104">
+        <f t="shared" si="47"/>
         <v>1907.1</v>
       </c>
       <c r="H36" s="104">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1958.3</v>
       </c>
       <c r="I36" s="104">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1978.3751090344099</v>
       </c>
       <c r="J36" s="104">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>2007.0179878174299</v>
       </c>
-      <c r="K36" s="149">
-        <f t="shared" si="46"/>
+      <c r="K36" s="104">
+        <f t="shared" si="47"/>
         <v>2033.6981662082601</v>
       </c>
       <c r="L36" s="104"/>
@@ -24928,23 +24952,23 @@
         <v>4.8999999999978172E-2</v>
       </c>
       <c r="G37" s="150">
-        <f t="shared" ref="G37:K37" si="47">G35-G36</f>
+        <f t="shared" ref="G37:K37" si="48">G35-G36</f>
         <v>-34.161000000000058</v>
       </c>
       <c r="H37" s="217">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-27.260999999999967</v>
       </c>
       <c r="I37" s="217">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-27.540460525652634</v>
       </c>
       <c r="J37" s="217">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-27.939190811356866</v>
       </c>
       <c r="K37" s="150">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-28.310598840325156</v>
       </c>
       <c r="L37" s="217">
@@ -25126,31 +25150,31 @@
         <v>#REF!</v>
       </c>
       <c r="E42" s="104">
-        <f t="shared" ref="E42:K42" si="48">D13</f>
+        <f>E13</f>
         <v>54.2</v>
       </c>
       <c r="F42" s="104">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="F42:K42" si="49">F13</f>
         <v>90.2</v>
       </c>
-      <c r="G42" s="149">
-        <f t="shared" si="48"/>
+      <c r="G42" s="104">
+        <f t="shared" si="49"/>
         <v>95.9</v>
       </c>
       <c r="H42" s="104">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>95.9</v>
       </c>
       <c r="I42" s="104">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>96.883099094316506</v>
       </c>
       <c r="J42" s="104">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>98.285770837814496</v>
       </c>
-      <c r="K42" s="149">
-        <f t="shared" si="48"/>
+      <c r="K42" s="104">
+        <f t="shared" si="49"/>
         <v>99.592327089502007</v>
       </c>
       <c r="L42" s="104"/>
@@ -25180,23 +25204,23 @@
         <v>0</v>
       </c>
       <c r="G43" s="150">
-        <f t="shared" ref="G43:K43" si="49">G41-G42</f>
+        <f t="shared" ref="G43:K43" si="50">G41-G42</f>
         <v>-4.3825959008611193</v>
       </c>
       <c r="H43" s="217">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-1.9565613146719585</v>
       </c>
       <c r="I43" s="217">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-1.9766185999319248</v>
       </c>
       <c r="J43" s="217">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-2.0052360480081859</v>
       </c>
       <c r="K43" s="150">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-2.0318925382843958</v>
       </c>
       <c r="L43" s="217">
@@ -25356,67 +25380,67 @@
         <v>1470.9965270419164</v>
       </c>
       <c r="L47" s="104">
-        <f t="shared" ref="L47:AA47" si="50">K47*(1+L49)</f>
+        <f t="shared" ref="L47:AA47" si="51">K47*(1+L49)</f>
         <v>1502.3965830074721</v>
       </c>
       <c r="M47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1533.7966389730275</v>
       </c>
       <c r="N47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1565.1966949385935</v>
       </c>
       <c r="O47" s="149">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1578.5108335772657</v>
       </c>
       <c r="P47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1591.8249722159278</v>
       </c>
       <c r="Q47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1605.1391108545999</v>
       </c>
       <c r="R47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1618.4532494932719</v>
       </c>
       <c r="S47" s="149">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1629.4283263923351</v>
       </c>
       <c r="T47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1640.4034032913987</v>
       </c>
       <c r="U47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1651.3784801904515</v>
       </c>
       <c r="V47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1662.3535570895151</v>
       </c>
       <c r="W47" s="149">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1703.3144246897598</v>
       </c>
       <c r="X47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1744.2752922900149</v>
       </c>
       <c r="Y47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1785.2361598902596</v>
       </c>
       <c r="Z47" s="104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1826.1970274905045</v>
       </c>
       <c r="AA47" s="149">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1856.7252504367495</v>
       </c>
       <c r="AB47" s="95"/>
@@ -25430,95 +25454,95 @@
         <v>#REF!</v>
       </c>
       <c r="E48" s="104">
-        <f t="shared" ref="E48:AA48" si="51">D14</f>
+        <f>E14</f>
         <v>1336.74</v>
       </c>
       <c r="F48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="F48:AA48" si="52">F14</f>
         <v>1328.7719999999999</v>
       </c>
-      <c r="G48" s="149">
-        <f t="shared" si="51"/>
+      <c r="G48" s="104">
+        <f t="shared" si="52"/>
         <v>1372.7929999999999</v>
       </c>
       <c r="H48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1403.2629999999999</v>
       </c>
       <c r="I48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1394.63952711825</v>
       </c>
-      <c r="J48" s="223">
-        <f t="shared" si="51"/>
+      <c r="J48" s="104">
+        <f t="shared" si="52"/>
         <v>1386.0160542364999</v>
       </c>
-      <c r="K48" s="149">
-        <f t="shared" si="51"/>
+      <c r="K48" s="104">
+        <f t="shared" si="52"/>
         <v>1416.24742986613</v>
       </c>
       <c r="L48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1446.4788054957501</v>
       </c>
       <c r="M48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1476.7101811253699</v>
       </c>
       <c r="N48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1506.941556755</v>
       </c>
-      <c r="O48" s="149">
-        <f t="shared" si="51"/>
+      <c r="O48" s="104">
+        <f t="shared" si="52"/>
         <v>1519.7601557667999</v>
       </c>
       <c r="P48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1532.5787547785901</v>
       </c>
       <c r="Q48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1545.3973537903901</v>
       </c>
       <c r="R48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1558.21595280219</v>
       </c>
-      <c r="S48" s="149">
-        <f t="shared" si="51"/>
+      <c r="S48" s="104">
+        <f t="shared" si="52"/>
         <v>1568.7825477363999</v>
       </c>
       <c r="T48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1579.34914267061</v>
       </c>
       <c r="U48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1589.9157376048099</v>
       </c>
       <c r="V48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1600.48233253902</v>
       </c>
-      <c r="W48" s="149">
-        <f t="shared" si="51"/>
+      <c r="W48" s="104">
+        <f t="shared" si="52"/>
         <v>1639.9186754518</v>
       </c>
       <c r="X48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1679.35501836459</v>
       </c>
       <c r="Y48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1718.79136127737</v>
       </c>
       <c r="Z48" s="104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1758.22770419015</v>
       </c>
-      <c r="AA48" s="149">
-        <f t="shared" si="51"/>
+      <c r="AA48" s="104">
+        <f t="shared" si="52"/>
         <v>1787.6196955994999</v>
       </c>
       <c r="AB48" s="95"/>
@@ -25535,71 +25559,71 @@
       <c r="I49" s="242"/>
       <c r="J49" s="242"/>
       <c r="K49" s="246">
-        <f t="shared" ref="K49" si="52">(K48/J48)-1</f>
+        <f t="shared" ref="K49" si="53">(K48/J48)-1</f>
         <v>2.1811706680615162E-2</v>
       </c>
       <c r="L49" s="230">
-        <f t="shared" ref="L49" si="53">(L48/K48)-1</f>
+        <f t="shared" ref="L49" si="54">(L48/K48)-1</f>
         <v>2.1346111556564518E-2</v>
       </c>
       <c r="M49" s="230">
-        <f t="shared" ref="M49" si="54">(M48/L48)-1</f>
+        <f t="shared" ref="M49" si="55">(M48/L48)-1</f>
         <v>2.0899978288488441E-2</v>
       </c>
       <c r="N49" s="230">
-        <f t="shared" ref="N49" si="55">(N48/M48)-1</f>
+        <f t="shared" ref="N49" si="56">(N48/M48)-1</f>
         <v>2.0472111600525089E-2</v>
       </c>
       <c r="O49" s="246">
-        <f t="shared" ref="O49" si="56">(O48/N48)-1</f>
+        <f t="shared" ref="O49" si="57">(O48/N48)-1</f>
         <v>8.5063677183361275E-3</v>
       </c>
       <c r="P49" s="230">
-        <f t="shared" ref="P49" si="57">(P48/O48)-1</f>
+        <f t="shared" ref="P49" si="58">(P48/O48)-1</f>
         <v>8.4346197412463741E-3</v>
       </c>
       <c r="Q49" s="230">
-        <f t="shared" ref="Q49" si="58">(Q48/P48)-1</f>
+        <f t="shared" ref="Q49" si="59">(Q48/P48)-1</f>
         <v>8.3640719746580494E-3</v>
       </c>
       <c r="R49" s="230">
-        <f t="shared" ref="R49" si="59">(R48/Q48)-1</f>
+        <f t="shared" ref="R49" si="60">(R48/Q48)-1</f>
         <v>8.2946945524138282E-3</v>
       </c>
       <c r="S49" s="246">
-        <f t="shared" ref="S49" si="60">(S48/R48)-1</f>
+        <f t="shared" ref="S49" si="61">(S48/R48)-1</f>
         <v>6.781213422444754E-3</v>
       </c>
       <c r="T49" s="230">
-        <f t="shared" ref="T49" si="61">(T48/S48)-1</f>
+        <f t="shared" ref="T49" si="62">(T48/S48)-1</f>
         <v>6.7355382997196234E-3</v>
       </c>
       <c r="U49" s="230">
-        <f t="shared" ref="U49" si="62">(U48/T48)-1</f>
+        <f t="shared" ref="U49" si="63">(U48/T48)-1</f>
         <v>6.6904743534619282E-3</v>
       </c>
       <c r="V49" s="230">
-        <f t="shared" ref="V49" si="63">(V48/U48)-1</f>
+        <f t="shared" ref="V49" si="64">(V48/U48)-1</f>
         <v>6.6460093980380552E-3</v>
       </c>
       <c r="W49" s="246">
-        <f t="shared" ref="W49" si="64">(W48/V48)-1</f>
+        <f t="shared" ref="W49" si="65">(W48/V48)-1</f>
         <v>2.4640286313075244E-2</v>
       </c>
       <c r="X49" s="230">
-        <f t="shared" ref="X49" si="65">(X48/W48)-1</f>
+        <f t="shared" ref="X49" si="66">(X48/W48)-1</f>
         <v>2.4047743039407266E-2</v>
       </c>
       <c r="Y49" s="230">
-        <f t="shared" ref="Y49" si="66">(Y48/X48)-1</f>
+        <f t="shared" ref="Y49" si="67">(Y48/X48)-1</f>
         <v>2.3483029187708171E-2</v>
       </c>
       <c r="Z49" s="230">
-        <f t="shared" ref="Z49" si="67">(Z48/Y48)-1</f>
+        <f t="shared" ref="Z49" si="68">(Z48/Y48)-1</f>
         <v>2.2944229184088893E-2</v>
       </c>
       <c r="AA49" s="246">
-        <f t="shared" ref="AA49" si="68">(AA48/Z48)-1</f>
+        <f t="shared" ref="AA49" si="69">(AA48/Z48)-1</f>
         <v>1.6716828735722888E-2</v>
       </c>
       <c r="AB49" s="243"/>
@@ -25611,91 +25635,91 @@
       <c r="D50" s="103"/>
       <c r="E50" s="217"/>
       <c r="F50" s="217">
-        <f t="shared" ref="F50" si="69">F47-F48</f>
+        <f t="shared" ref="F50" si="70">F47-F48</f>
         <v>3.3000000000129148E-2</v>
       </c>
       <c r="G50" s="150">
-        <f t="shared" ref="G50" si="70">G47-G48</f>
+        <f t="shared" ref="G50" si="71">G47-G48</f>
         <v>-5.9999999998581188E-3</v>
       </c>
       <c r="H50" s="217">
-        <f t="shared" ref="H50" si="71">H47-H48</f>
+        <f t="shared" ref="H50" si="72">H47-H48</f>
         <v>4.0000000001327862E-3</v>
       </c>
       <c r="I50" s="217">
-        <f t="shared" ref="I50" si="72">I47-I48</f>
+        <f t="shared" ref="I50" si="73">I47-I48</f>
         <v>21.90016870089994</v>
       </c>
       <c r="J50" s="239">
-        <f t="shared" ref="J50" si="73">J47-J48</f>
+        <f t="shared" ref="J50" si="74">J47-J48</f>
         <v>53.580416839850386</v>
       </c>
       <c r="K50" s="150">
-        <f t="shared" ref="K50:AA50" si="74">K47-K48</f>
+        <f t="shared" ref="K50:AA50" si="75">K47-K48</f>
         <v>54.749097175786346</v>
       </c>
       <c r="L50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>55.917777511722079</v>
       </c>
       <c r="M50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>57.086457847657584</v>
       </c>
       <c r="N50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>58.255138183593544</v>
       </c>
       <c r="O50" s="150">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>58.750677810465731</v>
       </c>
       <c r="P50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>59.246217437337691</v>
       </c>
       <c r="Q50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>59.741757064209878</v>
       </c>
       <c r="R50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>60.237296691081838</v>
       </c>
       <c r="S50" s="150">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>60.645778655935146</v>
       </c>
       <c r="T50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>61.054260620788682</v>
       </c>
       <c r="U50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>61.462742585641536</v>
       </c>
       <c r="V50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>61.871224550495072</v>
       </c>
       <c r="W50" s="150">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>63.395749237959762</v>
       </c>
       <c r="X50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>64.920273925424908</v>
       </c>
       <c r="Y50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>66.444798612889599</v>
       </c>
       <c r="Z50" s="217">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>67.969323300354517</v>
       </c>
       <c r="AA50" s="150">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>69.105554837249656</v>
       </c>
       <c r="AB50" s="244"/>
@@ -25814,63 +25838,63 @@
         <v>1684.5361789840949</v>
       </c>
       <c r="M54" s="104">
-        <f t="shared" ref="M54:AA54" si="75">L54*(1+M56)</f>
+        <f t="shared" ref="M54:AA54" si="76">L54*(1+M56)</f>
         <v>1678.2135536535579</v>
       </c>
       <c r="N54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1660.1984622255854</v>
       </c>
       <c r="O54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1681.5863017890024</v>
       </c>
       <c r="P54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1692.7375632632791</v>
       </c>
       <c r="Q54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1696.6630226959769</v>
       </c>
       <c r="R54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1692.281066197442</v>
       </c>
       <c r="S54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1700.8418499326938</v>
       </c>
       <c r="T54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1710.4578514658454</v>
       </c>
       <c r="U54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1719.6335883595932</v>
       </c>
       <c r="V54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1729.4009197745108</v>
       </c>
       <c r="W54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1769.6074835511222</v>
       </c>
       <c r="X54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1803.5824136795466</v>
       </c>
       <c r="Y54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1829.732881983369</v>
       </c>
       <c r="Z54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1848.8141695445154</v>
       </c>
       <c r="AA54" s="104">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1857.7181132918261</v>
       </c>
       <c r="AB54" s="95"/>
@@ -25884,95 +25908,95 @@
         <v>#REF!</v>
       </c>
       <c r="E55" s="104">
-        <f t="shared" ref="E55:AA55" si="76">D15</f>
+        <f>E15</f>
         <v>1828.5</v>
       </c>
       <c r="F55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" ref="F55:AA55" si="77">F15</f>
         <v>1861.4</v>
       </c>
-      <c r="G55" s="149">
-        <f t="shared" si="76"/>
+      <c r="G55" s="104">
+        <f t="shared" si="77"/>
         <v>1756.2</v>
       </c>
       <c r="H55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1808.7</v>
       </c>
       <c r="I55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1629.3563571043301</v>
       </c>
       <c r="J55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1501.6652887165701</v>
       </c>
-      <c r="K55" s="263">
-        <f t="shared" si="76"/>
+      <c r="K55" s="104">
+        <f t="shared" si="77"/>
         <v>1514.2729452476999</v>
       </c>
       <c r="L55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1515.61502429495</v>
       </c>
       <c r="M55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1509.9264163187599</v>
       </c>
       <c r="N55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1493.71783405563</v>
       </c>
-      <c r="O55" s="149">
-        <f t="shared" si="76"/>
+      <c r="O55" s="104">
+        <f t="shared" si="77"/>
         <v>1512.9609535468801</v>
       </c>
       <c r="P55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1522.99399388232</v>
       </c>
       <c r="Q55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1526.52581787499</v>
       </c>
       <c r="R55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1522.58327322214</v>
       </c>
-      <c r="S55" s="149">
-        <f t="shared" si="76"/>
+      <c r="S55" s="104">
+        <f t="shared" si="77"/>
         <v>1530.28560256998</v>
       </c>
       <c r="T55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1538.9373350641299</v>
       </c>
       <c r="U55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1547.1929515766401</v>
       </c>
       <c r="V55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1555.9808389633299</v>
       </c>
-      <c r="W55" s="149">
-        <f t="shared" si="76"/>
+      <c r="W55" s="104">
+        <f t="shared" si="77"/>
         <v>1592.1555871790999</v>
       </c>
       <c r="X55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1622.7235946783901</v>
       </c>
       <c r="Y55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1646.251758186</v>
       </c>
       <c r="Z55" s="104">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1663.41962105019</v>
       </c>
-      <c r="AA55" s="149">
-        <f t="shared" si="76"/>
+      <c r="AA55" s="104">
+        <f t="shared" si="77"/>
         <v>1671.4306991660901</v>
       </c>
       <c r="AB55" s="95"/>
@@ -25990,67 +26014,67 @@
       <c r="J56" s="242"/>
       <c r="K56" s="246"/>
       <c r="L56" s="230">
-        <f t="shared" ref="L56" si="77">(L55/K55)-1</f>
+        <f t="shared" ref="L56" si="78">(L55/K55)-1</f>
         <v>8.8628608961283106E-4</v>
       </c>
       <c r="M56" s="230">
-        <f t="shared" ref="M56" si="78">(M55/L55)-1</f>
+        <f t="shared" ref="M56" si="79">(M55/L55)-1</f>
         <v>-3.7533330595190817E-3</v>
       </c>
       <c r="N56" s="230">
-        <f t="shared" ref="N56" si="79">(N55/M55)-1</f>
+        <f t="shared" ref="N56" si="80">(N55/M55)-1</f>
         <v>-1.0734683550107649E-2</v>
       </c>
       <c r="O56" s="246">
-        <f t="shared" ref="O56" si="80">(O55/N55)-1</f>
+        <f t="shared" ref="O56" si="81">(O55/N55)-1</f>
         <v>1.2882700502411915E-2</v>
       </c>
       <c r="P56" s="230">
-        <f t="shared" ref="P56" si="81">(P55/O55)-1</f>
+        <f t="shared" ref="P56" si="82">(P55/O55)-1</f>
         <v>6.6313940964035645E-3</v>
       </c>
       <c r="Q56" s="230">
-        <f t="shared" ref="Q56" si="82">(Q55/P55)-1</f>
+        <f t="shared" ref="Q56" si="83">(Q55/P55)-1</f>
         <v>2.3190006046360789E-3</v>
       </c>
       <c r="R56" s="230">
-        <f t="shared" ref="R56" si="83">(R55/Q55)-1</f>
+        <f t="shared" ref="R56" si="84">(R55/Q55)-1</f>
         <v>-2.5826911059639857E-3</v>
       </c>
       <c r="S56" s="246">
-        <f t="shared" ref="S56" si="84">(S55/R55)-1</f>
+        <f t="shared" ref="S56" si="85">(S55/R55)-1</f>
         <v>5.0587245264688274E-3</v>
       </c>
       <c r="T56" s="230">
-        <f t="shared" ref="T56" si="85">(T55/S55)-1</f>
+        <f t="shared" ref="T56" si="86">(T55/S55)-1</f>
         <v>5.6536717588011598E-3</v>
       </c>
       <c r="U56" s="230">
-        <f t="shared" ref="U56" si="86">(U55/T55)-1</f>
+        <f t="shared" ref="U56" si="87">(U55/T55)-1</f>
         <v>5.3644916686397259E-3</v>
       </c>
       <c r="V56" s="230">
-        <f t="shared" ref="V56" si="87">(V55/U55)-1</f>
+        <f t="shared" ref="V56" si="88">(V55/U55)-1</f>
         <v>5.6798910425068794E-3</v>
       </c>
       <c r="W56" s="246">
-        <f t="shared" ref="W56" si="88">(W55/V55)-1</f>
+        <f t="shared" ref="W56" si="89">(W55/V55)-1</f>
         <v>2.3248839130867172E-2</v>
       </c>
       <c r="X56" s="230">
-        <f t="shared" ref="X56" si="89">(X55/W55)-1</f>
+        <f t="shared" ref="X56" si="90">(X55/W55)-1</f>
         <v>1.9199133392138412E-2</v>
       </c>
       <c r="Y56" s="230">
-        <f t="shared" ref="Y56" si="90">(Y55/X55)-1</f>
+        <f t="shared" ref="Y56" si="91">(Y55/X55)-1</f>
         <v>1.4499181243662784E-2</v>
       </c>
       <c r="Z56" s="230">
-        <f t="shared" ref="Z56" si="91">(Z55/Y55)-1</f>
+        <f t="shared" ref="Z56" si="92">(Z55/Y55)-1</f>
         <v>1.0428455294776651E-2</v>
       </c>
       <c r="AA56" s="246">
-        <f t="shared" ref="AA56" si="92">(AA55/Z55)-1</f>
+        <f t="shared" ref="AA56" si="93">(AA55/Z55)-1</f>
         <v>4.8160295902017758E-3</v>
       </c>
       <c r="AB56" s="243"/>
@@ -26062,91 +26086,91 @@
       <c r="D57" s="103"/>
       <c r="E57" s="217"/>
       <c r="F57" s="217">
-        <f t="shared" ref="F57" si="93">F54-F55</f>
+        <f t="shared" ref="F57" si="94">F54-F55</f>
         <v>604.60100000000011</v>
       </c>
       <c r="G57" s="150">
-        <f t="shared" ref="G57" si="94">G54-G55</f>
+        <f t="shared" ref="G57" si="95">G54-G55</f>
         <v>271.59299999999985</v>
       </c>
       <c r="H57" s="217">
-        <f t="shared" ref="H57" si="95">H54-H55</f>
+        <f t="shared" ref="H57" si="96">H54-H55</f>
         <v>1309.4238025000002</v>
       </c>
       <c r="I57" s="217">
-        <f t="shared" ref="I57" si="96">I54-I55</f>
+        <f t="shared" ref="I57" si="97">I54-I55</f>
         <v>245.49251687691981</v>
       </c>
       <c r="J57" s="217">
-        <f t="shared" ref="J57" si="97">J54-J55</f>
+        <f t="shared" ref="J57" si="98">J54-J55</f>
         <v>184.80221870982064</v>
       </c>
       <c r="K57" s="264">
-        <f t="shared" ref="K57" si="98">K54-K55</f>
+        <f t="shared" ref="K57" si="99">K54-K55</f>
         <v>168.77157479008633</v>
       </c>
       <c r="L57" s="217">
-        <f t="shared" ref="L57:AA57" si="99">L54-L55</f>
+        <f t="shared" ref="L57:AA57" si="100">L54-L55</f>
         <v>168.92115468914494</v>
       </c>
       <c r="M57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>168.28713733479799</v>
       </c>
       <c r="N57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>166.48062816995548</v>
       </c>
       <c r="O57" s="150">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>168.6253482421223</v>
       </c>
       <c r="P57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>169.74356938095912</v>
       </c>
       <c r="Q57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>170.13720482098688</v>
       </c>
       <c r="R57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>169.69779297530204</v>
       </c>
       <c r="S57" s="150">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>170.55624736271375</v>
       </c>
       <c r="T57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>171.52051640171544</v>
       </c>
       <c r="U57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>172.44063678295311</v>
       </c>
       <c r="V57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>173.42008081118092</v>
       </c>
       <c r="W57" s="150">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>177.45189637202225</v>
       </c>
       <c r="X57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>180.85881900115646</v>
       </c>
       <c r="Y57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>183.48112379736904</v>
       </c>
       <c r="Z57" s="217">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>185.39454849432536</v>
       </c>
       <c r="AA57" s="150">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>186.28741412573595</v>
       </c>
       <c r="AB57" s="244"/>
@@ -26288,47 +26312,47 @@
         <v>78.79947651486961</v>
       </c>
       <c r="Q61" s="231">
-        <f t="shared" ref="Q61:AA61" si="100">P61*(1+Q63)</f>
+        <f t="shared" ref="Q61:AA61" si="101">P61*(1+Q63)</f>
         <v>79.164740930401138</v>
       </c>
       <c r="R61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>79.5335062828227</v>
       </c>
       <c r="S61" s="247">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>79.905772572134268</v>
       </c>
       <c r="T61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>80.280372819372673</v>
       </c>
       <c r="U61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>80.654195080635461</v>
       </c>
       <c r="V61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>81.029184320861646</v>
       </c>
       <c r="W61" s="247">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>81.404951547063447</v>
       </c>
       <c r="X61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>81.780329780277256</v>
       </c>
       <c r="Y61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>82.151040097637818</v>
       </c>
       <c r="Z61" s="231">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>82.519027464083777</v>
       </c>
       <c r="AA61" s="247">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v>82.884291879615319</v>
       </c>
       <c r="AB61" s="95"/>
@@ -26342,95 +26366,95 @@
         <v>#REF!</v>
       </c>
       <c r="E62" s="104">
-        <f t="shared" ref="E62:AA62" si="101">D16</f>
+        <f>E16</f>
         <v>1085.9000000000001</v>
       </c>
       <c r="F62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" ref="F62:AA62" si="102">F16</f>
         <v>1212.9000000000001</v>
       </c>
-      <c r="G62" s="149">
-        <f t="shared" si="101"/>
+      <c r="G62" s="104">
+        <f t="shared" si="102"/>
         <v>609.79999999999995</v>
       </c>
       <c r="H62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>402.3</v>
       </c>
       <c r="I62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>404.18538158623397</v>
       </c>
       <c r="J62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>406.11408156777497</v>
       </c>
-      <c r="K62" s="149">
-        <f t="shared" si="101"/>
+      <c r="K62" s="104">
+        <f t="shared" si="102"/>
         <v>408.08197438316603</v>
       </c>
-      <c r="L62" s="223">
-        <f t="shared" si="101"/>
+      <c r="L62" s="104">
+        <f t="shared" si="102"/>
         <v>410.07255778657401</v>
       </c>
       <c r="M62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>412.05076450561</v>
       </c>
       <c r="N62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>413.998029513711</v>
       </c>
-      <c r="O62" s="149">
-        <f t="shared" si="101"/>
+      <c r="O62" s="104">
+        <f t="shared" si="102"/>
         <v>415.93291783743899</v>
       </c>
       <c r="P62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>417.86368059970903</v>
       </c>
       <c r="Q62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>419.80063170416599</v>
       </c>
       <c r="R62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>421.75614783518301</v>
       </c>
-      <c r="S62" s="149">
-        <f t="shared" si="101"/>
+      <c r="S62" s="104">
+        <f t="shared" si="102"/>
         <v>423.73022899275998</v>
       </c>
       <c r="T62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>425.71668683471103</v>
       </c>
       <c r="U62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>427.69901911520401</v>
       </c>
       <c r="V62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>429.68753973788398</v>
       </c>
-      <c r="W62" s="149">
-        <f t="shared" si="101"/>
+      <c r="W62" s="104">
+        <f t="shared" si="102"/>
         <v>431.68018592202202</v>
       </c>
       <c r="X62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>433.67076932543</v>
       </c>
       <c r="Y62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>435.63659936009202</v>
       </c>
       <c r="Z62" s="104">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>437.58798992965097</v>
       </c>
-      <c r="AA62" s="149">
-        <f t="shared" si="101"/>
+      <c r="AA62" s="104">
+        <f t="shared" si="102"/>
         <v>439.524941034108</v>
       </c>
       <c r="AB62" s="95"/>
@@ -26449,63 +26473,63 @@
       <c r="K63" s="229"/>
       <c r="L63" s="230"/>
       <c r="M63" s="230">
-        <f t="shared" ref="M63:AA63" si="102">(M62/L62)-1</f>
+        <f t="shared" ref="M63:AA63" si="103">(M62/L62)-1</f>
         <v>4.8240407251674E-3</v>
       </c>
       <c r="N63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.7257890916363454E-3</v>
       </c>
       <c r="O63" s="246">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6736655389416626E-3</v>
       </c>
       <c r="P63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6420051875399881E-3</v>
       </c>
       <c r="Q63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6353660162019583E-3</v>
       </c>
       <c r="R63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6582019733478752E-3</v>
       </c>
       <c r="S63" s="246">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6806221265762726E-3</v>
       </c>
       <c r="T63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6880248470189123E-3</v>
       </c>
       <c r="U63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6564589592013039E-3</v>
       </c>
       <c r="V63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6493457637422075E-3</v>
       </c>
       <c r="W63" s="246">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.637430690574762E-3</v>
       </c>
       <c r="X63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.6112457053277822E-3</v>
       </c>
       <c r="Y63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.5330010083912686E-3</v>
       </c>
       <c r="Z63" s="230">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.4793999687477992E-3</v>
       </c>
       <c r="AA63" s="246">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>4.4264265679878623E-3</v>
       </c>
       <c r="AB63" s="243"/>
@@ -26521,87 +26545,87 @@
         <v>0.57999999999992724</v>
       </c>
       <c r="G64" s="150">
-        <f t="shared" ref="G64:AA64" si="103">G61-G62</f>
+        <f t="shared" ref="G64:AA64" si="104">G61-G62</f>
         <v>0.73599999999999</v>
       </c>
       <c r="H64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>2.5539999999999736</v>
       </c>
       <c r="I64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>443.1982017470994</v>
       </c>
       <c r="J64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-298.69716490110829</v>
       </c>
       <c r="K64" s="150">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-305.33172438316603</v>
       </c>
       <c r="L64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-332.74230778657397</v>
       </c>
       <c r="M64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-334.34747023032264</v>
       </c>
       <c r="N64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-335.92752585795324</v>
       </c>
       <c r="O64" s="150">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-337.49753875913751</v>
       </c>
       <c r="P64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-339.06420408483939</v>
       </c>
       <c r="Q64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-340.63589077376486</v>
       </c>
       <c r="R64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-342.2226415523603</v>
       </c>
       <c r="S64" s="150">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-343.82445642062572</v>
       </c>
       <c r="T64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-345.43631401533833</v>
       </c>
       <c r="U64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-347.04482403456853</v>
       </c>
       <c r="V64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-348.65835541702234</v>
       </c>
       <c r="W64" s="150">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-350.27523437495859</v>
       </c>
       <c r="X64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-351.89043954515273</v>
       </c>
       <c r="Y64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-353.48555926245422</v>
       </c>
       <c r="Z64" s="217">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-355.06896246556721</v>
       </c>
       <c r="AA64" s="150">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>-356.64064915449268</v>
       </c>
       <c r="AB64" s="217"/>
@@ -26746,35 +26770,35 @@
         <v>330.50545802602733</v>
       </c>
       <c r="T68" s="248">
-        <f t="shared" ref="T68:AA68" si="104">S68*(1+T70)</f>
+        <f t="shared" ref="T68:AA68" si="105">S68*(1+T70)</f>
         <v>333.78582925174538</v>
       </c>
       <c r="U68" s="248">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>337.09010427322568</v>
       </c>
       <c r="V68" s="248">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>340.43479411501323</v>
       </c>
       <c r="W68" s="249">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>343.81583546649915</v>
       </c>
       <c r="X68" s="248">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>347.21186736980997</v>
       </c>
       <c r="Y68" s="248">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>350.62708384827226</v>
       </c>
       <c r="Z68" s="248">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>354.05853395040117</v>
       </c>
       <c r="AA68" s="249">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>357.51747852385301</v>
       </c>
       <c r="AB68" s="95"/>
@@ -26788,95 +26812,95 @@
         <v>#REF!</v>
       </c>
       <c r="E69" s="104">
-        <f t="shared" ref="E69:AA69" si="105">D17</f>
+        <f>E17</f>
         <v>884.26</v>
       </c>
       <c r="F69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" ref="F69:AA69" si="106">F17</f>
         <v>242.12799999999999</v>
       </c>
-      <c r="G69" s="149">
-        <f t="shared" si="105"/>
+      <c r="G69" s="104">
+        <f t="shared" si="106"/>
         <v>225.90700000000001</v>
       </c>
       <c r="H69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>260.73700000000002</v>
       </c>
       <c r="I69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>255.59948840017799</v>
       </c>
       <c r="J69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>254.55541346215</v>
       </c>
-      <c r="K69" s="149">
-        <f t="shared" si="105"/>
+      <c r="K69" s="104">
+        <f t="shared" si="106"/>
         <v>256.89572380491899</v>
       </c>
       <c r="L69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>259.47104592492298</v>
       </c>
       <c r="M69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>261.94028245643398</v>
       </c>
       <c r="N69" s="104">
-        <f t="shared" si="105"/>
+        <f t="shared" si="106"/>
         <v>264.42386516359801</v>
       </c>
-      <c r="O69" s="149">
-        <f t="shared" si="105"/>
+      <c r="O69" s="104">
+        <f t="shared" si="106"/>
         <v>266.96509198785299</v>
       </c>
-      <c r="P69" s="231">
-        <f t="shared" si="105"/>
+      <c r="P69" s="104">
+        <f t="shared" si="106"/>
         <v>269.50680093709798</v>
       </c>
-      <c r="Q69" s="231">
-        <f t="shared" si="105"/>
+      <c r="Q69" s="104">
+        <f t="shared" si="106"/>
         <v>272.09622896230098</v>
       </c>
-      <c r="R69" s="231">
-        <f t="shared" si="105"/>
+      <c r="R69" s="104">
+        <f t="shared" si="106"/>
         <v>274.73279727509299</v>
       </c>
-      <c r="S69" s="245">
-        <f t="shared" si="105"/>
+      <c r="S69" s="104">
+        <f t="shared" si="106"/>
         <v>277.43299355096599</v>
       </c>
-      <c r="T69" s="231">
-        <f t="shared" si="105"/>
+      <c r="T69" s="104">
+        <f t="shared" si="106"/>
         <v>280.18660377739002</v>
       </c>
-      <c r="U69" s="231">
-        <f t="shared" si="105"/>
+      <c r="U69" s="104">
+        <f t="shared" si="106"/>
         <v>282.96027933542803</v>
       </c>
-      <c r="V69" s="231">
-        <f t="shared" si="105"/>
+      <c r="V69" s="104">
+        <f t="shared" si="106"/>
         <v>285.76787991439801</v>
       </c>
-      <c r="W69" s="247">
-        <f t="shared" si="105"/>
+      <c r="W69" s="104">
+        <f t="shared" si="106"/>
         <v>288.60599468885499</v>
       </c>
-      <c r="X69" s="231">
-        <f t="shared" si="105"/>
+      <c r="X69" s="104">
+        <f t="shared" si="106"/>
         <v>291.45669283695003</v>
       </c>
-      <c r="Y69" s="231">
-        <f t="shared" si="105"/>
+      <c r="Y69" s="104">
+        <f t="shared" si="106"/>
         <v>294.32349490703803</v>
       </c>
-      <c r="Z69" s="231">
-        <f t="shared" si="105"/>
+      <c r="Z69" s="104">
+        <f t="shared" si="106"/>
         <v>297.203923810513</v>
       </c>
-      <c r="AA69" s="247">
-        <f t="shared" si="105"/>
+      <c r="AA69" s="104">
+        <f t="shared" si="106"/>
         <v>300.10743213158901</v>
       </c>
       <c r="AB69" s="95"/>
@@ -26899,47 +26923,47 @@
       <c r="O70" s="246"/>
       <c r="P70" s="230"/>
       <c r="Q70" s="230">
-        <f t="shared" ref="Q70" si="106">(Q69/P69)-1</f>
+        <f t="shared" ref="Q70" si="107">(Q69/P69)-1</f>
         <v>9.6080247926930706E-3</v>
       </c>
       <c r="R70" s="230">
-        <f t="shared" ref="R70" si="107">(R69/Q69)-1</f>
+        <f t="shared" ref="R70" si="108">(R69/Q69)-1</f>
         <v>9.6898377564700322E-3</v>
       </c>
       <c r="S70" s="246">
-        <f t="shared" ref="S70" si="108">(S69/R69)-1</f>
+        <f t="shared" ref="S70" si="109">(S69/R69)-1</f>
         <v>9.8284453208885569E-3</v>
       </c>
       <c r="T70" s="230">
-        <f t="shared" ref="T70" si="109">(T69/S69)-1</f>
+        <f t="shared" ref="T70" si="110">(T69/S69)-1</f>
         <v>9.9253163482091455E-3</v>
       </c>
       <c r="U70" s="230">
-        <f t="shared" ref="U70" si="110">(U69/T69)-1</f>
+        <f t="shared" ref="U70" si="111">(U69/T69)-1</f>
         <v>9.8993867681187453E-3</v>
       </c>
       <c r="V70" s="230">
-        <f t="shared" ref="V70" si="111">(V69/U69)-1</f>
+        <f t="shared" ref="V70" si="112">(V69/U69)-1</f>
         <v>9.9222427457452689E-3</v>
       </c>
       <c r="W70" s="246">
-        <f t="shared" ref="W70" si="112">(W69/V69)-1</f>
+        <f t="shared" ref="W70" si="113">(W69/V69)-1</f>
         <v>9.9315387555352075E-3</v>
       </c>
       <c r="X70" s="230">
-        <f t="shared" ref="X70" si="113">(X69/W69)-1</f>
+        <f t="shared" ref="X70" si="114">(X69/W69)-1</f>
         <v>9.877473789719371E-3</v>
       </c>
       <c r="Y70" s="230">
-        <f t="shared" ref="Y70" si="114">(Y69/X69)-1</f>
+        <f t="shared" ref="Y70" si="115">(Y69/X69)-1</f>
         <v>9.8361167903999736E-3</v>
       </c>
       <c r="Z70" s="230">
-        <f t="shared" ref="Z70" si="115">(Z69/Y69)-1</f>
+        <f t="shared" ref="Z70" si="116">(Z69/Y69)-1</f>
         <v>9.7866087937856783E-3</v>
       </c>
       <c r="AA70" s="246">
-        <f t="shared" ref="AA70" si="116">(AA69/Z69)-1</f>
+        <f t="shared" ref="AA70" si="117">(AA69/Z69)-1</f>
         <v>9.7694144944304728E-3</v>
       </c>
       <c r="AB70" s="243"/>
@@ -26955,87 +26979,87 @@
         <v>49.271999999999991</v>
       </c>
       <c r="G71" s="150">
-        <f t="shared" ref="G71:K71" si="117">G68-G69</f>
+        <f t="shared" ref="G71:K71" si="118">G68-G69</f>
         <v>68.244</v>
       </c>
       <c r="H71" s="217">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>61.90180399999997</v>
       </c>
       <c r="I71" s="217">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>68.930270815822013</v>
       </c>
       <c r="J71" s="217">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>64.768464790714006</v>
       </c>
       <c r="K71" s="150">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>62.225449960956496</v>
       </c>
       <c r="L71" s="217">
-        <f t="shared" ref="L71:N71" si="118">L68-L69</f>
+        <f t="shared" ref="L71:N71" si="119">L68-L69</f>
         <v>50.450612536015967</v>
       </c>
       <c r="M71" s="217">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>48.785062638348734</v>
       </c>
       <c r="N71" s="217">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>47.108381311563846</v>
       </c>
       <c r="O71" s="150">
-        <f t="shared" ref="O71:AA71" si="119">O68-O69</f>
+        <f t="shared" ref="O71:AA71" si="120">O68-O69</f>
         <v>45.377283473209502</v>
       </c>
       <c r="P71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>43.648944025808703</v>
       </c>
       <c r="Q71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>58.409229063726343</v>
       </c>
       <c r="R71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>55.772660750934335</v>
       </c>
       <c r="S71" s="239">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>53.072464475061338</v>
       </c>
       <c r="T71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>53.599225474355364</v>
       </c>
       <c r="U71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>54.12982493779765</v>
       </c>
       <c r="V71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>54.666914200615224</v>
       </c>
       <c r="W71" s="251">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>55.20984077764416</v>
       </c>
       <c r="X71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>55.75517453285994</v>
       </c>
       <c r="Y71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>56.303588941234239</v>
       </c>
       <c r="Z71" s="250">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>56.854610139888166</v>
       </c>
       <c r="AA71" s="251">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>57.410046392264007</v>
       </c>
       <c r="AB71" s="244"/>
@@ -27096,7 +27120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M25" sqref="M25"/>
     </sheetView>
@@ -27219,7 +27243,7 @@
       </c>
       <c r="C3">
         <f t="array" ref="C3:C24">TRANSPOSE('add-ons calculations'!F31:AA31)</f>
-        <v>-33.023000000000025</v>
+        <v>185.97699999999998</v>
       </c>
       <c r="D3">
         <f t="array" ref="D3:D24">TRANSPOSE('add-ons calculations'!F37:AA37)</f>
@@ -27277,7 +27301,7 @@
         <v>-8.7680000000000007</v>
       </c>
       <c r="C4">
-        <v>-61.292000000000002</v>
+        <v>36.608000000000004</v>
       </c>
       <c r="D4">
         <v>-34.161000000000058</v>
@@ -27329,7 +27353,7 @@
         <v>-2.6000000000010459E-2</v>
       </c>
       <c r="C5">
-        <v>-10.88900000000001</v>
+        <v>60.010999999999996</v>
       </c>
       <c r="D5">
         <v>-27.260999999999967</v>
@@ -27382,7 +27406,7 @@
         <v>12.191000475937102</v>
       </c>
       <c r="C6">
-        <v>-31.404359752822046</v>
+        <v>41.205300797277943</v>
       </c>
       <c r="D6">
         <v>-27.540460525652634</v>
@@ -27437,7 +27461,7 @@
         <v>8.0446176857161049</v>
       </c>
       <c r="C7">
-        <v>-31.299870882672082</v>
+        <v>42.720344650758932</v>
       </c>
       <c r="D7">
         <v>-27.939190811356866</v>
@@ -27492,7 +27516,7 @@
         <v>7.459524934637102</v>
       </c>
       <c r="C8">
-        <v>-42.728540027182873</v>
+        <v>32.46624938209311</v>
       </c>
       <c r="D8">
         <v>-28.310598840325156</v>
@@ -27547,7 +27571,7 @@
         <v>6.8744321835571043</v>
       </c>
       <c r="C9">
-        <v>-54.017481243801626</v>
+        <v>22.370520514336363</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -27602,7 +27626,7 @@
         <v>47.937274032360733</v>
       </c>
       <c r="C10">
-        <v>-56.860234186327006</v>
+        <v>23.915633540108274</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -27657,7 +27681,7 @@
         <v>47.352181281280735</v>
       </c>
       <c r="C11">
-        <v>-59.4982734243018</v>
+        <v>25.347666673136104</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -27712,7 +27736,7 @@
         <v>49.24529837870972</v>
       </c>
       <c r="C12">
-        <v>-64.18782156080772</v>
+        <v>28.01951799620258</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -27767,7 +27791,7 @@
         <v>48.706029963479068</v>
       </c>
       <c r="C13">
-        <v>-68.649682849032899</v>
+        <v>30.565599506059044</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -27820,7 +27844,7 @@
         <v>48.166761548248445</v>
       </c>
       <c r="C14">
-        <v>-73.145039224524623</v>
+        <v>33.130183054574275</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -27872,7 +27896,7 @@
         <v>47.627493133017822</v>
       </c>
       <c r="C15">
-        <v>-77.637929717548047</v>
+        <v>35.693404497285769</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -27924,7 +27948,7 @@
         <v>47.909170525827761</v>
       </c>
       <c r="C16">
-        <v>-79.591929938656051</v>
+        <v>36.730219990317664</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -27976,7 +28000,7 @@
         <v>48.190847918637417</v>
       </c>
       <c r="C17">
-        <v>-81.64451473965164</v>
+        <v>37.821491699382307</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -28028,7 +28052,7 @@
         <v>48.472525311447043</v>
       </c>
       <c r="C18">
-        <v>-83.786721885999441</v>
+        <v>38.962269059386188</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -28080,7 +28104,7 @@
         <v>48.754202704256983</v>
       </c>
       <c r="C19">
-        <v>-85.803457748854214</v>
+        <v>40.033738508075317</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -28132,7 +28156,7 @@
         <v>49.478730408519283</v>
       </c>
       <c r="C20">
-        <v>-86.263002893230009</v>
+        <v>40.178170532473189</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -28184,7 +28208,7 @@
         <v>50.203258112781555</v>
       </c>
       <c r="C21">
-        <v>-86.713585803070657</v>
+        <v>40.317651991777097</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -28236,7 +28260,7 @@
         <v>50.927785817043855</v>
       </c>
       <c r="C22">
-        <v>-87.155206478375987</v>
+        <v>40.452182885987327</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -28288,7 +28312,7 @@
         <v>51.652313521306155</v>
       </c>
       <c r="C23">
-        <v>-87.596827153681318</v>
+        <v>40.586713780197385</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -28340,7 +28364,7 @@
         <v>52.373839507047563</v>
       </c>
       <c r="C24">
-        <v>-88.048091531449472</v>
+        <v>40.727024962454834</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -33479,6 +33503,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -33695,12 +33725,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -33711,6 +33735,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B484070-5C48-4F32-AF92-870650EA512F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33729,23 +33770,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
   <ds:schemaRefs>

</xml_diff>